<commit_message>
listen to my heart
</commit_message>
<xml_diff>
--- a/questionnaires/RBDstandardized_questionnaire_MAD_FR.xlsx
+++ b/questionnaires/RBDstandardized_questionnaire_MAD_FR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RBD_Resilience_guide_FR\questionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6E1DF8-D656-4E57-B47B-B68C0600E111}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BECFB2D-08D1-452E-AC92-63307BDF36B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1545" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="2" r:id="rId1"/>
@@ -1109,9 +1109,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T170"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="37" spans="1:16" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="37" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>61</v>
@@ -2152,7 +2152,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>

</xml_diff>